<commit_message>
Append record to Combined.xlsx
</commit_message>
<xml_diff>
--- a/data/Combined.xlsx
+++ b/data/Combined.xlsx
@@ -1565,7 +1565,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ59"/>
+  <dimension ref="A1:AJ60"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -8060,9 +8060,119 @@
         <v>Danpoo</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>DIFF</v>
+      </c>
+      <c r="B60" t="str">
+        <v>xyz</v>
+      </c>
+      <c r="C60" t="str">
+        <v>KLOPD3412</v>
+      </c>
+      <c r="D60" t="str">
+        <v>-</v>
+      </c>
+      <c r="E60" t="str">
+        <v>3</v>
+      </c>
+      <c r="F60" t="str">
+        <v>14</v>
+      </c>
+      <c r="G60" t="str">
+        <v>12</v>
+      </c>
+      <c r="H60" t="str">
+        <v>14</v>
+      </c>
+      <c r="I60" t="str">
+        <v>30x8x2.5</v>
+      </c>
+      <c r="J60" t="str">
+        <v>424</v>
+      </c>
+      <c r="K60" t="str">
+        <v>-</v>
+      </c>
+      <c r="L60" t="str">
+        <v>4</v>
+      </c>
+      <c r="M60" t="str">
+        <v>Black</v>
+      </c>
+      <c r="N60" t="str">
+        <v>Alloy steel</v>
+      </c>
+      <c r="O60" t="str">
+        <v>choice of screws or glue + Screw cap</v>
+      </c>
+      <c r="P60" t="str">
+        <v>-</v>
+      </c>
+      <c r="Q60" t="str">
+        <v>Danpoo</v>
+      </c>
+      <c r="R60" t="str">
+        <v>14.3</v>
+      </c>
+      <c r="S60" t="str">
+        <v>1</v>
+      </c>
+      <c r="T60" t="str">
+        <v>1452</v>
+      </c>
+      <c r="U60" t="str">
+        <v>100</v>
+      </c>
+      <c r="V60" t="str">
+        <v>14,854.08</v>
+      </c>
+      <c r="W60" t="str">
+        <v>5236</v>
+      </c>
+      <c r="X60" t="str">
+        <v>4</v>
+      </c>
+      <c r="Y60" t="str">
+        <v>133,172</v>
+      </c>
+      <c r="Z60" t="str">
+        <v>CN</v>
+      </c>
+      <c r="AA60" t="str">
+        <v>1425</v>
+      </c>
+      <c r="AB60" t="str">
+        <v>452</v>
+      </c>
+      <c r="AC60" t="str">
+        <v>474</v>
+      </c>
+      <c r="AD60" t="str">
+        <v>5</v>
+      </c>
+      <c r="AE60" t="str">
+        <v>MEISHIMEIQI US</v>
+      </c>
+      <c r="AF60" t="str">
+        <v>Home &amp; Kitchen</v>
+      </c>
+      <c r="AG60" t="str">
+        <v>Large and Bulky</v>
+      </c>
+      <c r="AH60" t="str">
+        <v>FBA</v>
+      </c>
+      <c r="AI60" t="str">
+        <v>2026-01-01</v>
+      </c>
+      <c r="AJ60" t="str">
+        <v>Danpoo</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AJ59"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AJ60"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>